<commit_message>
Modyfy Check_list and Test_case
</commit_message>
<xml_diff>
--- a/Check_list.xlsx
+++ b/Check_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Adel_sc\diplom\My_os\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8601922-1E79-4423-A2EE-B2DE58F6B705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E76AD6E-69EB-4AE6-8AD5-0DDEC7C91C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>Проверка</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>Отмена фильтрации новостей</t>
+  </si>
+  <si>
+    <t>Страница тематических цитат</t>
+  </si>
+  <si>
+    <t>Переход на страницу тематических цитат</t>
+  </si>
+  <si>
+    <t>Развернуть тематическую цитату</t>
   </si>
 </sst>
 </file>
@@ -500,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +797,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
@@ -796,7 +805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>35</v>
       </c>
@@ -804,7 +813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
@@ -812,7 +821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
@@ -820,7 +829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>38</v>
       </c>
@@ -828,7 +837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
@@ -836,12 +845,42 @@
         <v>10</v>
       </c>
     </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A16:I16"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A39:I39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>